<commit_message>
Reviewed metrics from Rui
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint1/Burndown chart.xlsx
+++ b/Project/Phase 2/Sprint1/Burndown chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="EsteLivro" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rui_j\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophia\Desktop\Sophia\Faculdade\ES\ganttprojectstable\Project\Phase 2\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CE8368-CA98-4814-A20F-394A88835D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E91336-CB84-445C-8B1E-F0D75DDF99A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4464" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -538,6 +538,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -567,24 +585,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,7 +611,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -673,7 +673,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RW"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -965,7 +965,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RW"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1048433599"/>
@@ -1049,7 +1049,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-RW"/>
+              <a:endParaRPr lang="pt-PT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1081,7 +1081,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-RW"/>
+            <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1048432767"/>
@@ -1124,7 +1124,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-RW"/>
+          <a:endParaRPr lang="pt-PT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1161,7 +1161,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-RW"/>
+      <a:endParaRPr lang="pt-PT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1770,7 +1770,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2072,41 +2072,45 @@
   <dimension ref="B1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="33" t="s">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="35"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
     </row>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="36"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="38"/>
+    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -2128,9 +2132,9 @@
         <v>44869</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="32"/>
-      <c r="C5" s="30"/>
+    <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="38"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
@@ -2150,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="22">
         <v>1</v>
       </c>
@@ -2176,11 +2180,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="27" t="s">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="19">
         <v>0</v>
       </c>
@@ -2205,11 +2209,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="26"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="11">
         <f>SUM(D6:D7)</f>
         <v>10</v>
@@ -2235,11 +2239,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+    <row r="9" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="24"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="13">
         <f>D8</f>
         <v>10</v>
@@ -2265,16 +2269,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the FINAL report
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint1/Burndown chart.xlsx
+++ b/Project/Phase 2/Sprint1/Burndown chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophia\Desktop\Sophia\Faculdade\ES\ganttprojectstable\Project\Phase 2\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E91336-CB84-445C-8B1E-F0D75DDF99A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E893F51-9A40-4A20-B170-E7F9B8652314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4464" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Sprint Burndown Chart</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Search possible funcionalities to implement</t>
+  </si>
+  <si>
+    <t>Day 5</t>
+  </si>
+  <si>
+    <t>Day 4</t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -332,17 +338,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -432,24 +427,65 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -460,7 +496,9 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -470,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -508,7 +546,7 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -526,25 +564,19 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -553,26 +585,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -585,6 +608,39 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,17 +735,27 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.8249830593172878E-2"/>
+          <c:y val="8.9495762448215346E-2"/>
+          <c:w val="0.92175016940682708"/>
+          <c:h val="0.78167290635546982"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$7:$C$7</c:f>
+              <c:f>'Burndown Chart'!$B$16:$C$16</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -710,28 +776,34 @@
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$7:$G$7</c:f>
+              <c:f>'Burndown Chart'!$D$16:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8D0E-4F8E-897D-5B1720B3868B}"/>
+              <c16:uniqueId val="{00000007-AE15-481E-B629-7B8708FDC1DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -744,7 +816,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
         <c:axId val="1048432767"/>
         <c:axId val="1048433599"/>
       </c:barChart>
@@ -756,11 +827,109 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$B$8:$C$8</c:f>
+              <c:f>'Burndown Chart'!$B$17:$C$17</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Remaining Effort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Burndown Chart'!$D$5:$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Day 0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burndown Chart'!$D$17:$I$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-AE15-481E-B629-7B8708FDC1DA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burndown Chart'!$B$18:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Ideal Burndown</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -775,25 +944,13 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Burndown Chart'!$D$5:$G$5</c:f>
+              <c:f>'Burndown Chart'!$D$5:$I$5</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Day 0</c:v>
                 </c:pt>
@@ -805,27 +962,39 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Day 3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$D$8:$G$8</c:f>
+              <c:f>'Burndown Chart'!$D$18:$I$18</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -833,81 +1002,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8D0E-4F8E-897D-5B1720B3868B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$B$9:$C$9</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Ideal Burndown</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:srgbClr val="00B050"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Burndown Chart'!$D$5:$G$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Day 0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Burndown Chart'!$D$9:$G$9</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8D0E-4F8E-897D-5B1720B3868B}"/>
+              <c16:uniqueId val="{00000006-AE15-481E-B629-7B8708FDC1DA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -979,7 +1074,7 @@
         <c:axId val="1048433599"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="31"/>
+          <c:max val="11"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1019,7 +1114,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Tasks</a:t>
+                  <a:t>Hours</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1087,7 +1182,6 @@
         <c:crossAx val="1048432767"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1173,13 +1267,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1733,26 +1824,28 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>7842</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>108697</xdr:rowOff>
+      <xdr:colOff>170330</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>681317</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>105336</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>71718</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>175935</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52BFCA64-3DDA-4711-BDFA-D2973C7C7C4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{058A3F66-F908-4505-8468-87FF0776DE25}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2069,10 +2162,10 @@
   <sheetPr codeName="Folha1">
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B1:I21"/>
+  <dimension ref="B1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2081,36 +2174,37 @@
     <col min="3" max="3" width="73.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="26"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="25"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="30" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -2133,8 +2227,8 @@
       </c>
     </row>
     <row r="5" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="38"/>
-      <c r="C5" s="36"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
@@ -2148,137 +2242,295 @@
         <v>7</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="22">
+    <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="19">
         <v>1</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="16">
-        <v>10</v>
-      </c>
-      <c r="E6" s="7">
         <v>1</v>
       </c>
+      <c r="E6" s="7"/>
       <c r="F6" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="19">
         <v>2</v>
       </c>
-      <c r="G6" s="9">
+      <c r="C7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="16">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9">
+        <v>1</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="19">
         <v>3</v>
       </c>
-      <c r="H6" s="9">
+      <c r="C8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="16">
         <v>1</v>
       </c>
-      <c r="I6" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="19">
-        <v>0</v>
-      </c>
-      <c r="E7" s="20">
-        <f>SUM(E6:E6)</f>
-        <v>1</v>
-      </c>
-      <c r="F7" s="20">
-        <f>SUM(F6:F6)</f>
-        <v>2</v>
-      </c>
-      <c r="G7" s="21">
-        <f>SUM(G6:G6)</f>
-        <v>3</v>
-      </c>
-      <c r="H7" s="21">
-        <f>SUM(H6:H6)</f>
-        <v>1</v>
-      </c>
-      <c r="I7" s="21">
-        <f>SUM(I6:I6)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="11">
-        <f>SUM(D6:D7)</f>
-        <v>10</v>
-      </c>
-      <c r="E8" s="12">
-        <f>D8-SUM(E6:E6)</f>
-        <v>9</v>
-      </c>
-      <c r="F8" s="10">
-        <f>E8-SUM(F6:F6)</f>
-        <v>7</v>
-      </c>
-      <c r="G8" s="18">
-        <f>F8-SUM(G6:G6)</f>
-        <v>4</v>
-      </c>
-      <c r="H8" s="18">
-        <f>G8-SUM(H6:H6)</f>
-        <v>3</v>
-      </c>
-      <c r="I8" s="18">
-        <f>H8-SUM(I6:I6)</f>
-        <v>0</v>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9">
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="19">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="19">
+        <v>5</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="16">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="19">
+        <v>6</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="16">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="19">
+        <v>7</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="19">
+        <v>8</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="16">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="19">
+        <v>9</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="16">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="34">
         <v>10</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="13">
-        <f>D8</f>
+      <c r="C15" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="36">
+        <v>1</v>
+      </c>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42">
+        <v>0</v>
+      </c>
+      <c r="E16" s="43">
+        <f>SUM(E6:E15)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="43">
+        <f>SUM(F6:F15)</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="44">
+        <f>SUM(G6:G15)</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="44">
+        <f>SUM(H6:H15)</f>
+        <v>3</v>
+      </c>
+      <c r="I16" s="44">
+        <f>SUM(I6:I15)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="11">
+        <f>SUM(D6:D16)</f>
         <v>10</v>
       </c>
-      <c r="E9" s="14">
-        <f>$D$9-($D$9/(COLUMNS(E5:I5))*COLUMNS(E5))</f>
+      <c r="E17" s="12">
+        <f>D17-E16</f>
+        <v>10</v>
+      </c>
+      <c r="F17" s="10">
+        <f>E17-F16</f>
+        <v>9</v>
+      </c>
+      <c r="G17" s="18">
+        <f>F17-G16</f>
         <v>8</v>
       </c>
-      <c r="F9" s="1">
-        <f>$D$9-($D$9/(COLUMNS(E5:I5))*COLUMNS(E5:F5))</f>
+      <c r="H17" s="18">
+        <f>G17-H16</f>
+        <v>5</v>
+      </c>
+      <c r="I17" s="18">
+        <f>H17-I16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="13">
+        <f>D17</f>
+        <v>10</v>
+      </c>
+      <c r="E18" s="14">
+        <f>$D$18-($D$18/(COLUMNS(E5:I5))*COLUMNS(E5))</f>
+        <v>8</v>
+      </c>
+      <c r="F18" s="1">
+        <f>$D$18-($D$18/(COLUMNS(E5:I5))*COLUMNS(E5:F5))</f>
         <v>6</v>
       </c>
-      <c r="G9" s="2">
-        <f>$D$9-($D$9/(COLUMNS(E5:I5))*COLUMNS(E5:G5))</f>
+      <c r="G18" s="2">
+        <f>$D$18-($D$18/(COLUMNS(E5:I5))*COLUMNS(E5:G5))</f>
         <v>4</v>
       </c>
-      <c r="H9" s="2">
-        <f>$D$9-($D$9/(COLUMNS(E5:I5))*COLUMNS(E5:H5))</f>
+      <c r="H18" s="2">
+        <f>$D$18-($D$18/(COLUMNS(E5:I5))*COLUMNS(E5:H5))</f>
         <v>2</v>
       </c>
-      <c r="I9" s="2">
-        <f>$D$9-($D$9/(COLUMNS(E5:I5))*COLUMNS(E5:I5))</f>
+      <c r="I18" s="2">
+        <f>$D$18-($D$18/(COLUMNS(E5:I5))*COLUMNS(E5:I5))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>